<commit_message>
changes to data to add a "structure" number
</commit_message>
<xml_diff>
--- a/raw_data/genotype_data.xlsx
+++ b/raw_data/genotype_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6183A58B-7B51-414F-A5E4-D91D434D23BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5FBC95-CCDF-9649-8C69-ACF955A9A7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="500" windowWidth="27240" windowHeight="13640" xr2:uid="{8655E8E0-4FE4-9C41-9F55-F43691CC9339}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="13640" xr2:uid="{8655E8E0-4FE4-9C41-9F55-F43691CC9339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="288">
   <si>
     <t>sample_id</t>
   </si>
@@ -495,6 +495,411 @@
   </si>
   <si>
     <t>structure_number</t>
+  </si>
+  <si>
+    <t>FBS_01</t>
+  </si>
+  <si>
+    <t>FBS_02</t>
+  </si>
+  <si>
+    <t>FBS_03</t>
+  </si>
+  <si>
+    <t>FBS_04</t>
+  </si>
+  <si>
+    <t>FBS_05</t>
+  </si>
+  <si>
+    <t>FBS_06</t>
+  </si>
+  <si>
+    <t>FBS_07</t>
+  </si>
+  <si>
+    <t>FBS_08</t>
+  </si>
+  <si>
+    <t>FBS_09</t>
+  </si>
+  <si>
+    <t>FBS_10</t>
+  </si>
+  <si>
+    <t>FBS_11</t>
+  </si>
+  <si>
+    <t>FBS_12</t>
+  </si>
+  <si>
+    <t>FBS_13</t>
+  </si>
+  <si>
+    <t>FBS_14</t>
+  </si>
+  <si>
+    <t>FBS_15</t>
+  </si>
+  <si>
+    <t>FBS_16</t>
+  </si>
+  <si>
+    <t>FBS_17</t>
+  </si>
+  <si>
+    <t>FBS_18</t>
+  </si>
+  <si>
+    <t>FBS_19</t>
+  </si>
+  <si>
+    <t>FBS_20</t>
+  </si>
+  <si>
+    <t>FBS_21</t>
+  </si>
+  <si>
+    <t>FBS_22</t>
+  </si>
+  <si>
+    <t>FBS_23</t>
+  </si>
+  <si>
+    <t>FBS_24</t>
+  </si>
+  <si>
+    <t>FBS_25</t>
+  </si>
+  <si>
+    <t>FBS_26</t>
+  </si>
+  <si>
+    <t>FBS_27</t>
+  </si>
+  <si>
+    <t>FBS_28</t>
+  </si>
+  <si>
+    <t>FBS_29</t>
+  </si>
+  <si>
+    <t>FBS_30</t>
+  </si>
+  <si>
+    <t>FBS_31</t>
+  </si>
+  <si>
+    <t>FBS_32</t>
+  </si>
+  <si>
+    <t>FBS_33</t>
+  </si>
+  <si>
+    <t>FBS_34</t>
+  </si>
+  <si>
+    <t>FBS_35</t>
+  </si>
+  <si>
+    <t>FBS_36</t>
+  </si>
+  <si>
+    <t>FBS_37</t>
+  </si>
+  <si>
+    <t>FBS_38</t>
+  </si>
+  <si>
+    <t>FBS_39</t>
+  </si>
+  <si>
+    <t>FBS_40</t>
+  </si>
+  <si>
+    <t>FBS_41</t>
+  </si>
+  <si>
+    <t>FBS_42</t>
+  </si>
+  <si>
+    <t>FBS_43</t>
+  </si>
+  <si>
+    <t>FBS_44</t>
+  </si>
+  <si>
+    <t>FBS_45</t>
+  </si>
+  <si>
+    <t>FBS_46</t>
+  </si>
+  <si>
+    <t>FER_01</t>
+  </si>
+  <si>
+    <t>FER_02</t>
+  </si>
+  <si>
+    <t>FER_03</t>
+  </si>
+  <si>
+    <t>FER_04</t>
+  </si>
+  <si>
+    <t>FER_05</t>
+  </si>
+  <si>
+    <t>FER_06</t>
+  </si>
+  <si>
+    <t>FER_07</t>
+  </si>
+  <si>
+    <t>FER_08</t>
+  </si>
+  <si>
+    <t>FER_09</t>
+  </si>
+  <si>
+    <t>FER_10</t>
+  </si>
+  <si>
+    <t>FER_11</t>
+  </si>
+  <si>
+    <t>FER_12</t>
+  </si>
+  <si>
+    <t>FER_13</t>
+  </si>
+  <si>
+    <t>FER_14</t>
+  </si>
+  <si>
+    <t>FER_15</t>
+  </si>
+  <si>
+    <t>FER_16</t>
+  </si>
+  <si>
+    <t>FER_17</t>
+  </si>
+  <si>
+    <t>FER_18</t>
+  </si>
+  <si>
+    <t>FER_19</t>
+  </si>
+  <si>
+    <t>FER_20</t>
+  </si>
+  <si>
+    <t>FER_21</t>
+  </si>
+  <si>
+    <t>FER_22</t>
+  </si>
+  <si>
+    <t>FER_23</t>
+  </si>
+  <si>
+    <t>FER_24</t>
+  </si>
+  <si>
+    <t>FER_25</t>
+  </si>
+  <si>
+    <t>FER_26</t>
+  </si>
+  <si>
+    <t>FER_27</t>
+  </si>
+  <si>
+    <t>FER_28</t>
+  </si>
+  <si>
+    <t>FER_29</t>
+  </si>
+  <si>
+    <t>FER_30</t>
+  </si>
+  <si>
+    <t>FER_31</t>
+  </si>
+  <si>
+    <t>FER_32</t>
+  </si>
+  <si>
+    <t>FER_33</t>
+  </si>
+  <si>
+    <t>FER_34</t>
+  </si>
+  <si>
+    <t>FER_35</t>
+  </si>
+  <si>
+    <t>FER_36</t>
+  </si>
+  <si>
+    <t>FER_37</t>
+  </si>
+  <si>
+    <t>FER_38</t>
+  </si>
+  <si>
+    <t>FER_39</t>
+  </si>
+  <si>
+    <t>FER_40</t>
+  </si>
+  <si>
+    <t>FER_41</t>
+  </si>
+  <si>
+    <t>FER_42</t>
+  </si>
+  <si>
+    <t>FER_43</t>
+  </si>
+  <si>
+    <t>FER_44</t>
+  </si>
+  <si>
+    <t>FER_45</t>
+  </si>
+  <si>
+    <t>FER_46</t>
+  </si>
+  <si>
+    <t>FER_47</t>
+  </si>
+  <si>
+    <t>FER_48</t>
+  </si>
+  <si>
+    <t>FER_49</t>
+  </si>
+  <si>
+    <t>FER_50</t>
+  </si>
+  <si>
+    <t>FER_51</t>
+  </si>
+  <si>
+    <t>FER_52</t>
+  </si>
+  <si>
+    <t>FER_53</t>
+  </si>
+  <si>
+    <t>FER_54</t>
+  </si>
+  <si>
+    <t>FER_55</t>
+  </si>
+  <si>
+    <t>FER_56</t>
+  </si>
+  <si>
+    <t>FER_57</t>
+  </si>
+  <si>
+    <t>FER_58</t>
+  </si>
+  <si>
+    <t>FER_59</t>
+  </si>
+  <si>
+    <t>FER_60</t>
+  </si>
+  <si>
+    <t>FER_61</t>
+  </si>
+  <si>
+    <t>FER_62</t>
+  </si>
+  <si>
+    <t>FER_63</t>
+  </si>
+  <si>
+    <t>FER_64</t>
+  </si>
+  <si>
+    <t>FER_65</t>
+  </si>
+  <si>
+    <t>FER_66</t>
+  </si>
+  <si>
+    <t>FER_68</t>
+  </si>
+  <si>
+    <t>FER_69</t>
+  </si>
+  <si>
+    <t>FER_70</t>
+  </si>
+  <si>
+    <t>GRSPB_31</t>
+  </si>
+  <si>
+    <t>GRSPB_32</t>
+  </si>
+  <si>
+    <t>GRSPB_33</t>
+  </si>
+  <si>
+    <t>GRSPB_34</t>
+  </si>
+  <si>
+    <t>GRSPB_35</t>
+  </si>
+  <si>
+    <t>GRSPB_36</t>
+  </si>
+  <si>
+    <t>GRSPB_37</t>
+  </si>
+  <si>
+    <t>GRSPB_39</t>
+  </si>
+  <si>
+    <t>GRSPB_41</t>
+  </si>
+  <si>
+    <t>GRSPB_44</t>
+  </si>
+  <si>
+    <t>GRSPB_46</t>
+  </si>
+  <si>
+    <t>GRSPB_49</t>
+  </si>
+  <si>
+    <t>TBLR_01</t>
+  </si>
+  <si>
+    <t>TBLR_02</t>
+  </si>
+  <si>
+    <t>TBLR_03</t>
+  </si>
+  <si>
+    <t>TBLR_04</t>
+  </si>
+  <si>
+    <t>TBLR_05</t>
+  </si>
+  <si>
+    <t>TBLR_06</t>
+  </si>
+  <si>
+    <t>TBLR_07</t>
+  </si>
+  <si>
+    <t>TBLR_08</t>
   </si>
 </sst>
 </file>
@@ -876,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BABEBB-635A-534D-90BA-1C6A4991D774}">
   <dimension ref="A1:AD136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,9 +1386,8 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="str">
-        <f>CONCATENATE(LEFT(A2,3),"_",RIGHT(A2,2))</f>
-        <v>FBS_01</v>
+      <c r="B2" t="s">
+        <v>153</v>
       </c>
       <c r="C2">
         <v>123</v>
@@ -1074,9 +1478,8 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B66" si="0">CONCATENATE(LEFT(A3,3),"_",RIGHT(A3,2))</f>
-        <v>FBS_02</v>
+      <c r="B3" t="s">
+        <v>154</v>
       </c>
       <c r="C3">
         <v>125</v>
@@ -1167,9 +1570,8 @@
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_03</v>
+      <c r="B4" t="s">
+        <v>155</v>
       </c>
       <c r="C4">
         <v>125</v>
@@ -1260,9 +1662,8 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_04</v>
+      <c r="B5" t="s">
+        <v>156</v>
       </c>
       <c r="C5">
         <v>123</v>
@@ -1353,9 +1754,8 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_05</v>
+      <c r="B6" t="s">
+        <v>157</v>
       </c>
       <c r="C6">
         <v>123</v>
@@ -1446,9 +1846,8 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_06</v>
+      <c r="B7" t="s">
+        <v>158</v>
       </c>
       <c r="C7">
         <v>123</v>
@@ -1539,9 +1938,8 @@
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_07</v>
+      <c r="B8" t="s">
+        <v>159</v>
       </c>
       <c r="C8">
         <v>131</v>
@@ -1632,9 +2030,8 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_08</v>
+      <c r="B9" t="s">
+        <v>160</v>
       </c>
       <c r="C9">
         <v>125</v>
@@ -1725,9 +2122,8 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_09</v>
+      <c r="B10" t="s">
+        <v>161</v>
       </c>
       <c r="C10">
         <v>123</v>
@@ -1818,9 +2214,8 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_10</v>
+      <c r="B11" t="s">
+        <v>162</v>
       </c>
       <c r="C11">
         <v>123</v>
@@ -1911,9 +2306,8 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_11</v>
+      <c r="B12" t="s">
+        <v>163</v>
       </c>
       <c r="C12">
         <v>123</v>
@@ -2004,9 +2398,8 @@
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_12</v>
+      <c r="B13" t="s">
+        <v>164</v>
       </c>
       <c r="C13">
         <v>123</v>
@@ -2097,9 +2490,8 @@
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_13</v>
+      <c r="B14" t="s">
+        <v>165</v>
       </c>
       <c r="C14">
         <v>131</v>
@@ -2190,9 +2582,8 @@
       <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_14</v>
+      <c r="B15" t="s">
+        <v>166</v>
       </c>
       <c r="C15">
         <v>123</v>
@@ -2283,9 +2674,8 @@
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_15</v>
+      <c r="B16" t="s">
+        <v>167</v>
       </c>
       <c r="C16">
         <v>125</v>
@@ -2376,9 +2766,8 @@
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_16</v>
+      <c r="B17" t="s">
+        <v>168</v>
       </c>
       <c r="C17">
         <v>123</v>
@@ -2469,9 +2858,8 @@
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_17</v>
+      <c r="B18" t="s">
+        <v>169</v>
       </c>
       <c r="C18">
         <v>125</v>
@@ -2562,9 +2950,8 @@
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_18</v>
+      <c r="B19" t="s">
+        <v>170</v>
       </c>
       <c r="C19">
         <v>125</v>
@@ -2655,9 +3042,8 @@
       <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_19</v>
+      <c r="B20" t="s">
+        <v>171</v>
       </c>
       <c r="C20">
         <v>123</v>
@@ -2748,9 +3134,8 @@
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_20</v>
+      <c r="B21" t="s">
+        <v>172</v>
       </c>
       <c r="C21">
         <v>125</v>
@@ -2841,9 +3226,8 @@
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_21</v>
+      <c r="B22" t="s">
+        <v>173</v>
       </c>
       <c r="C22">
         <v>123</v>
@@ -2934,9 +3318,8 @@
       <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_22</v>
+      <c r="B23" t="s">
+        <v>174</v>
       </c>
       <c r="C23">
         <v>129</v>
@@ -3027,9 +3410,8 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_23</v>
+      <c r="B24" t="s">
+        <v>175</v>
       </c>
       <c r="C24">
         <v>123</v>
@@ -3120,9 +3502,8 @@
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_24</v>
+      <c r="B25" t="s">
+        <v>176</v>
       </c>
       <c r="C25">
         <v>123</v>
@@ -3213,9 +3594,8 @@
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_25</v>
+      <c r="B26" t="s">
+        <v>177</v>
       </c>
       <c r="C26">
         <v>123</v>
@@ -3306,9 +3686,8 @@
       <c r="A27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_26</v>
+      <c r="B27" t="s">
+        <v>178</v>
       </c>
       <c r="C27">
         <v>125</v>
@@ -3399,9 +3778,8 @@
       <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_27</v>
+      <c r="B28" t="s">
+        <v>179</v>
       </c>
       <c r="C28">
         <v>125</v>
@@ -3492,9 +3870,8 @@
       <c r="A29" t="s">
         <v>42</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_28</v>
+      <c r="B29" t="s">
+        <v>180</v>
       </c>
       <c r="C29">
         <v>129</v>
@@ -3585,9 +3962,8 @@
       <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_29</v>
+      <c r="B30" t="s">
+        <v>181</v>
       </c>
       <c r="C30">
         <v>129</v>
@@ -3678,9 +4054,8 @@
       <c r="A31" t="s">
         <v>44</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_30</v>
+      <c r="B31" t="s">
+        <v>182</v>
       </c>
       <c r="C31">
         <v>123</v>
@@ -3771,9 +4146,8 @@
       <c r="A32" t="s">
         <v>45</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_31</v>
+      <c r="B32" t="s">
+        <v>183</v>
       </c>
       <c r="C32">
         <v>123</v>
@@ -3864,9 +4238,8 @@
       <c r="A33" t="s">
         <v>46</v>
       </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_32</v>
+      <c r="B33" t="s">
+        <v>184</v>
       </c>
       <c r="C33">
         <v>123</v>
@@ -3957,9 +4330,8 @@
       <c r="A34" t="s">
         <v>47</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_33</v>
+      <c r="B34" t="s">
+        <v>185</v>
       </c>
       <c r="C34">
         <v>123</v>
@@ -4050,9 +4422,8 @@
       <c r="A35" t="s">
         <v>48</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_34</v>
+      <c r="B35" t="s">
+        <v>186</v>
       </c>
       <c r="C35">
         <v>123</v>
@@ -4143,9 +4514,8 @@
       <c r="A36" t="s">
         <v>49</v>
       </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_35</v>
+      <c r="B36" t="s">
+        <v>187</v>
       </c>
       <c r="C36">
         <v>125</v>
@@ -4236,9 +4606,8 @@
       <c r="A37" t="s">
         <v>50</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_36</v>
+      <c r="B37" t="s">
+        <v>188</v>
       </c>
       <c r="C37">
         <v>123</v>
@@ -4329,9 +4698,8 @@
       <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_37</v>
+      <c r="B38" t="s">
+        <v>189</v>
       </c>
       <c r="C38">
         <v>129</v>
@@ -4422,9 +4790,8 @@
       <c r="A39" t="s">
         <v>52</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_38</v>
+      <c r="B39" t="s">
+        <v>190</v>
       </c>
       <c r="C39">
         <v>129</v>
@@ -4515,9 +4882,8 @@
       <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_39</v>
+      <c r="B40" t="s">
+        <v>191</v>
       </c>
       <c r="C40">
         <v>123</v>
@@ -4608,9 +4974,8 @@
       <c r="A41" t="s">
         <v>54</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_40</v>
+      <c r="B41" t="s">
+        <v>192</v>
       </c>
       <c r="C41">
         <v>123</v>
@@ -4701,9 +5066,8 @@
       <c r="A42" t="s">
         <v>55</v>
       </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_41</v>
+      <c r="B42" t="s">
+        <v>193</v>
       </c>
       <c r="C42">
         <v>129</v>
@@ -4794,9 +5158,8 @@
       <c r="A43" t="s">
         <v>56</v>
       </c>
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_42</v>
+      <c r="B43" t="s">
+        <v>194</v>
       </c>
       <c r="C43">
         <v>123</v>
@@ -4887,9 +5250,8 @@
       <c r="A44" t="s">
         <v>57</v>
       </c>
-      <c r="B44" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_43</v>
+      <c r="B44" t="s">
+        <v>195</v>
       </c>
       <c r="C44">
         <v>123</v>
@@ -4980,9 +5342,8 @@
       <c r="A45" t="s">
         <v>58</v>
       </c>
-      <c r="B45" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_44</v>
+      <c r="B45" t="s">
+        <v>196</v>
       </c>
       <c r="C45">
         <v>123</v>
@@ -5073,9 +5434,8 @@
       <c r="A46" t="s">
         <v>59</v>
       </c>
-      <c r="B46" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_45</v>
+      <c r="B46" t="s">
+        <v>197</v>
       </c>
       <c r="C46">
         <v>123</v>
@@ -5166,9 +5526,8 @@
       <c r="A47" t="s">
         <v>60</v>
       </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>FBS_46</v>
+      <c r="B47" t="s">
+        <v>198</v>
       </c>
       <c r="C47">
         <v>123</v>
@@ -5259,9 +5618,8 @@
       <c r="A48" t="s">
         <v>61</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_01</v>
+      <c r="B48" t="s">
+        <v>199</v>
       </c>
       <c r="C48">
         <v>123</v>
@@ -5352,9 +5710,8 @@
       <c r="A49" t="s">
         <v>62</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_02</v>
+      <c r="B49" t="s">
+        <v>200</v>
       </c>
       <c r="C49">
         <v>123</v>
@@ -5445,9 +5802,8 @@
       <c r="A50" t="s">
         <v>63</v>
       </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_03</v>
+      <c r="B50" t="s">
+        <v>201</v>
       </c>
       <c r="C50">
         <v>129</v>
@@ -5538,9 +5894,8 @@
       <c r="A51" t="s">
         <v>64</v>
       </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_04</v>
+      <c r="B51" t="s">
+        <v>202</v>
       </c>
       <c r="C51">
         <v>123</v>
@@ -5631,9 +5986,8 @@
       <c r="A52" t="s">
         <v>65</v>
       </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_05</v>
+      <c r="B52" t="s">
+        <v>203</v>
       </c>
       <c r="C52">
         <v>123</v>
@@ -5724,9 +6078,8 @@
       <c r="A53" t="s">
         <v>66</v>
       </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_06</v>
+      <c r="B53" t="s">
+        <v>204</v>
       </c>
       <c r="C53">
         <v>123</v>
@@ -5817,9 +6170,8 @@
       <c r="A54" t="s">
         <v>67</v>
       </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_07</v>
+      <c r="B54" t="s">
+        <v>205</v>
       </c>
       <c r="C54">
         <v>123</v>
@@ -5910,9 +6262,8 @@
       <c r="A55" t="s">
         <v>68</v>
       </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_08</v>
+      <c r="B55" t="s">
+        <v>206</v>
       </c>
       <c r="C55">
         <v>129</v>
@@ -6003,9 +6354,8 @@
       <c r="A56" t="s">
         <v>69</v>
       </c>
-      <c r="B56" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_09</v>
+      <c r="B56" t="s">
+        <v>207</v>
       </c>
       <c r="C56">
         <v>123</v>
@@ -6096,9 +6446,8 @@
       <c r="A57" t="s">
         <v>70</v>
       </c>
-      <c r="B57" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_10</v>
+      <c r="B57" t="s">
+        <v>208</v>
       </c>
       <c r="C57">
         <v>123</v>
@@ -6189,9 +6538,8 @@
       <c r="A58" t="s">
         <v>71</v>
       </c>
-      <c r="B58" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_11</v>
+      <c r="B58" t="s">
+        <v>209</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>150</v>
@@ -6282,9 +6630,8 @@
       <c r="A59" t="s">
         <v>72</v>
       </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_12</v>
+      <c r="B59" t="s">
+        <v>210</v>
       </c>
       <c r="C59">
         <v>125</v>
@@ -6375,9 +6722,8 @@
       <c r="A60" t="s">
         <v>73</v>
       </c>
-      <c r="B60" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_13</v>
+      <c r="B60" t="s">
+        <v>211</v>
       </c>
       <c r="C60">
         <v>123</v>
@@ -6468,9 +6814,8 @@
       <c r="A61" t="s">
         <v>74</v>
       </c>
-      <c r="B61" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_14</v>
+      <c r="B61" t="s">
+        <v>212</v>
       </c>
       <c r="C61">
         <v>123</v>
@@ -6561,9 +6906,8 @@
       <c r="A62" t="s">
         <v>75</v>
       </c>
-      <c r="B62" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_15</v>
+      <c r="B62" t="s">
+        <v>213</v>
       </c>
       <c r="C62">
         <v>129</v>
@@ -6654,9 +6998,8 @@
       <c r="A63" t="s">
         <v>76</v>
       </c>
-      <c r="B63" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_16</v>
+      <c r="B63" t="s">
+        <v>214</v>
       </c>
       <c r="C63">
         <v>123</v>
@@ -6747,9 +7090,8 @@
       <c r="A64" t="s">
         <v>77</v>
       </c>
-      <c r="B64" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_17</v>
+      <c r="B64" t="s">
+        <v>215</v>
       </c>
       <c r="C64">
         <v>123</v>
@@ -6840,9 +7182,8 @@
       <c r="A65" t="s">
         <v>78</v>
       </c>
-      <c r="B65" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_18</v>
+      <c r="B65" t="s">
+        <v>216</v>
       </c>
       <c r="C65">
         <v>123</v>
@@ -6933,9 +7274,8 @@
       <c r="A66" t="s">
         <v>79</v>
       </c>
-      <c r="B66" t="str">
-        <f t="shared" si="0"/>
-        <v>FER_19</v>
+      <c r="B66" t="s">
+        <v>217</v>
       </c>
       <c r="C66">
         <v>129</v>
@@ -7026,9 +7366,8 @@
       <c r="A67" t="s">
         <v>80</v>
       </c>
-      <c r="B67" t="str">
-        <f t="shared" ref="B67:B116" si="1">CONCATENATE(LEFT(A67,3),"_",RIGHT(A67,2))</f>
-        <v>FER_20</v>
+      <c r="B67" t="s">
+        <v>218</v>
       </c>
       <c r="C67">
         <v>123</v>
@@ -7119,9 +7458,8 @@
       <c r="A68" t="s">
         <v>81</v>
       </c>
-      <c r="B68" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_21</v>
+      <c r="B68" t="s">
+        <v>219</v>
       </c>
       <c r="C68">
         <v>123</v>
@@ -7212,9 +7550,8 @@
       <c r="A69" t="s">
         <v>82</v>
       </c>
-      <c r="B69" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_22</v>
+      <c r="B69" t="s">
+        <v>220</v>
       </c>
       <c r="C69">
         <v>123</v>
@@ -7305,9 +7642,8 @@
       <c r="A70" t="s">
         <v>83</v>
       </c>
-      <c r="B70" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_23</v>
+      <c r="B70" t="s">
+        <v>221</v>
       </c>
       <c r="C70">
         <v>123</v>
@@ -7398,9 +7734,8 @@
       <c r="A71" t="s">
         <v>84</v>
       </c>
-      <c r="B71" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_24</v>
+      <c r="B71" t="s">
+        <v>222</v>
       </c>
       <c r="C71">
         <v>123</v>
@@ -7491,9 +7826,8 @@
       <c r="A72" t="s">
         <v>85</v>
       </c>
-      <c r="B72" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_25</v>
+      <c r="B72" t="s">
+        <v>223</v>
       </c>
       <c r="C72">
         <v>123</v>
@@ -7584,9 +7918,8 @@
       <c r="A73" t="s">
         <v>86</v>
       </c>
-      <c r="B73" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_26</v>
+      <c r="B73" t="s">
+        <v>224</v>
       </c>
       <c r="C73">
         <v>129</v>
@@ -7677,9 +8010,8 @@
       <c r="A74" t="s">
         <v>87</v>
       </c>
-      <c r="B74" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_27</v>
+      <c r="B74" t="s">
+        <v>225</v>
       </c>
       <c r="C74">
         <v>123</v>
@@ -7770,9 +8102,8 @@
       <c r="A75" t="s">
         <v>88</v>
       </c>
-      <c r="B75" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_28</v>
+      <c r="B75" t="s">
+        <v>226</v>
       </c>
       <c r="C75">
         <v>123</v>
@@ -7863,9 +8194,8 @@
       <c r="A76" t="s">
         <v>89</v>
       </c>
-      <c r="B76" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_29</v>
+      <c r="B76" t="s">
+        <v>227</v>
       </c>
       <c r="C76">
         <v>123</v>
@@ -7956,9 +8286,8 @@
       <c r="A77" t="s">
         <v>90</v>
       </c>
-      <c r="B77" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_30</v>
+      <c r="B77" t="s">
+        <v>228</v>
       </c>
       <c r="C77">
         <v>123</v>
@@ -8049,9 +8378,8 @@
       <c r="A78" t="s">
         <v>91</v>
       </c>
-      <c r="B78" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_31</v>
+      <c r="B78" t="s">
+        <v>229</v>
       </c>
       <c r="C78">
         <v>123</v>
@@ -8142,9 +8470,8 @@
       <c r="A79" t="s">
         <v>92</v>
       </c>
-      <c r="B79" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_32</v>
+      <c r="B79" t="s">
+        <v>230</v>
       </c>
       <c r="C79">
         <v>125</v>
@@ -8235,9 +8562,8 @@
       <c r="A80" t="s">
         <v>93</v>
       </c>
-      <c r="B80" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_33</v>
+      <c r="B80" t="s">
+        <v>231</v>
       </c>
       <c r="C80">
         <v>125</v>
@@ -8328,9 +8654,8 @@
       <c r="A81" t="s">
         <v>94</v>
       </c>
-      <c r="B81" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_34</v>
+      <c r="B81" t="s">
+        <v>232</v>
       </c>
       <c r="C81">
         <v>123</v>
@@ -8421,9 +8746,8 @@
       <c r="A82" t="s">
         <v>95</v>
       </c>
-      <c r="B82" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_35</v>
+      <c r="B82" t="s">
+        <v>233</v>
       </c>
       <c r="C82">
         <v>129</v>
@@ -8514,9 +8838,8 @@
       <c r="A83" t="s">
         <v>96</v>
       </c>
-      <c r="B83" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_36</v>
+      <c r="B83" t="s">
+        <v>234</v>
       </c>
       <c r="C83">
         <v>125</v>
@@ -8607,9 +8930,8 @@
       <c r="A84" t="s">
         <v>97</v>
       </c>
-      <c r="B84" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_37</v>
+      <c r="B84" t="s">
+        <v>235</v>
       </c>
       <c r="C84">
         <v>129</v>
@@ -8700,9 +9022,8 @@
       <c r="A85" t="s">
         <v>98</v>
       </c>
-      <c r="B85" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_38</v>
+      <c r="B85" t="s">
+        <v>236</v>
       </c>
       <c r="C85">
         <v>123</v>
@@ -8793,9 +9114,8 @@
       <c r="A86" t="s">
         <v>99</v>
       </c>
-      <c r="B86" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_39</v>
+      <c r="B86" t="s">
+        <v>237</v>
       </c>
       <c r="C86">
         <v>123</v>
@@ -8886,9 +9206,8 @@
       <c r="A87" t="s">
         <v>100</v>
       </c>
-      <c r="B87" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_40</v>
+      <c r="B87" t="s">
+        <v>238</v>
       </c>
       <c r="C87">
         <v>129</v>
@@ -8979,9 +9298,8 @@
       <c r="A88" t="s">
         <v>101</v>
       </c>
-      <c r="B88" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_41</v>
+      <c r="B88" t="s">
+        <v>239</v>
       </c>
       <c r="C88">
         <v>123</v>
@@ -9072,9 +9390,8 @@
       <c r="A89" t="s">
         <v>102</v>
       </c>
-      <c r="B89" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_42</v>
+      <c r="B89" t="s">
+        <v>240</v>
       </c>
       <c r="C89">
         <v>123</v>
@@ -9165,9 +9482,8 @@
       <c r="A90" t="s">
         <v>103</v>
       </c>
-      <c r="B90" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_43</v>
+      <c r="B90" t="s">
+        <v>241</v>
       </c>
       <c r="C90">
         <v>123</v>
@@ -9258,9 +9574,8 @@
       <c r="A91" t="s">
         <v>104</v>
       </c>
-      <c r="B91" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_44</v>
+      <c r="B91" t="s">
+        <v>242</v>
       </c>
       <c r="C91">
         <v>123</v>
@@ -9351,9 +9666,8 @@
       <c r="A92" t="s">
         <v>105</v>
       </c>
-      <c r="B92" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_45</v>
+      <c r="B92" t="s">
+        <v>243</v>
       </c>
       <c r="C92">
         <v>125</v>
@@ -9444,9 +9758,8 @@
       <c r="A93" t="s">
         <v>106</v>
       </c>
-      <c r="B93" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_46</v>
+      <c r="B93" t="s">
+        <v>244</v>
       </c>
       <c r="C93">
         <v>129</v>
@@ -9537,9 +9850,8 @@
       <c r="A94" t="s">
         <v>107</v>
       </c>
-      <c r="B94" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_47</v>
+      <c r="B94" t="s">
+        <v>245</v>
       </c>
       <c r="C94">
         <v>123</v>
@@ -9630,9 +9942,8 @@
       <c r="A95" t="s">
         <v>108</v>
       </c>
-      <c r="B95" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_48</v>
+      <c r="B95" t="s">
+        <v>246</v>
       </c>
       <c r="C95">
         <v>123</v>
@@ -9723,9 +10034,8 @@
       <c r="A96" t="s">
         <v>109</v>
       </c>
-      <c r="B96" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_49</v>
+      <c r="B96" t="s">
+        <v>247</v>
       </c>
       <c r="C96">
         <v>129</v>
@@ -9816,9 +10126,8 @@
       <c r="A97" t="s">
         <v>110</v>
       </c>
-      <c r="B97" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_50</v>
+      <c r="B97" t="s">
+        <v>248</v>
       </c>
       <c r="C97">
         <v>125</v>
@@ -9909,9 +10218,8 @@
       <c r="A98" t="s">
         <v>111</v>
       </c>
-      <c r="B98" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_51</v>
+      <c r="B98" t="s">
+        <v>249</v>
       </c>
       <c r="C98">
         <v>123</v>
@@ -10002,9 +10310,8 @@
       <c r="A99" t="s">
         <v>112</v>
       </c>
-      <c r="B99" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_52</v>
+      <c r="B99" t="s">
+        <v>250</v>
       </c>
       <c r="C99">
         <v>123</v>
@@ -10095,9 +10402,8 @@
       <c r="A100" t="s">
         <v>113</v>
       </c>
-      <c r="B100" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_53</v>
+      <c r="B100" t="s">
+        <v>251</v>
       </c>
       <c r="C100">
         <v>123</v>
@@ -10188,9 +10494,8 @@
       <c r="A101" t="s">
         <v>114</v>
       </c>
-      <c r="B101" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_54</v>
+      <c r="B101" t="s">
+        <v>252</v>
       </c>
       <c r="C101">
         <v>123</v>
@@ -10281,9 +10586,8 @@
       <c r="A102" t="s">
         <v>115</v>
       </c>
-      <c r="B102" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_55</v>
+      <c r="B102" t="s">
+        <v>253</v>
       </c>
       <c r="C102">
         <v>129</v>
@@ -10374,9 +10678,8 @@
       <c r="A103" t="s">
         <v>116</v>
       </c>
-      <c r="B103" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_56</v>
+      <c r="B103" t="s">
+        <v>254</v>
       </c>
       <c r="C103">
         <v>129</v>
@@ -10467,9 +10770,8 @@
       <c r="A104" t="s">
         <v>117</v>
       </c>
-      <c r="B104" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_57</v>
+      <c r="B104" t="s">
+        <v>255</v>
       </c>
       <c r="C104">
         <v>123</v>
@@ -10560,9 +10862,8 @@
       <c r="A105" t="s">
         <v>118</v>
       </c>
-      <c r="B105" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_58</v>
+      <c r="B105" t="s">
+        <v>256</v>
       </c>
       <c r="C105">
         <v>123</v>
@@ -10653,9 +10954,8 @@
       <c r="A106" t="s">
         <v>119</v>
       </c>
-      <c r="B106" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_59</v>
+      <c r="B106" t="s">
+        <v>257</v>
       </c>
       <c r="C106">
         <v>123</v>
@@ -10746,9 +11046,8 @@
       <c r="A107" t="s">
         <v>120</v>
       </c>
-      <c r="B107" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_60</v>
+      <c r="B107" t="s">
+        <v>258</v>
       </c>
       <c r="C107">
         <v>125</v>
@@ -10839,9 +11138,8 @@
       <c r="A108" t="s">
         <v>121</v>
       </c>
-      <c r="B108" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_61</v>
+      <c r="B108" t="s">
+        <v>259</v>
       </c>
       <c r="C108">
         <v>125</v>
@@ -10932,9 +11230,8 @@
       <c r="A109" t="s">
         <v>122</v>
       </c>
-      <c r="B109" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_62</v>
+      <c r="B109" t="s">
+        <v>260</v>
       </c>
       <c r="C109">
         <v>123</v>
@@ -11025,9 +11322,8 @@
       <c r="A110" t="s">
         <v>123</v>
       </c>
-      <c r="B110" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_63</v>
+      <c r="B110" t="s">
+        <v>261</v>
       </c>
       <c r="C110">
         <v>123</v>
@@ -11118,9 +11414,8 @@
       <c r="A111" t="s">
         <v>124</v>
       </c>
-      <c r="B111" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_64</v>
+      <c r="B111" t="s">
+        <v>262</v>
       </c>
       <c r="C111">
         <v>123</v>
@@ -11211,9 +11506,8 @@
       <c r="A112" t="s">
         <v>125</v>
       </c>
-      <c r="B112" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_65</v>
+      <c r="B112" t="s">
+        <v>263</v>
       </c>
       <c r="C112">
         <v>123</v>
@@ -11304,9 +11598,8 @@
       <c r="A113" t="s">
         <v>126</v>
       </c>
-      <c r="B113" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_66</v>
+      <c r="B113" t="s">
+        <v>264</v>
       </c>
       <c r="C113">
         <v>125</v>
@@ -11397,9 +11690,8 @@
       <c r="A114" t="s">
         <v>127</v>
       </c>
-      <c r="B114" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_68</v>
+      <c r="B114" t="s">
+        <v>265</v>
       </c>
       <c r="C114">
         <v>123</v>
@@ -11490,9 +11782,8 @@
       <c r="A115" t="s">
         <v>128</v>
       </c>
-      <c r="B115" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_69</v>
+      <c r="B115" t="s">
+        <v>266</v>
       </c>
       <c r="C115">
         <v>123</v>
@@ -11583,9 +11874,8 @@
       <c r="A116" t="s">
         <v>129</v>
       </c>
-      <c r="B116" t="str">
-        <f t="shared" si="1"/>
-        <v>FER_70</v>
+      <c r="B116" t="s">
+        <v>267</v>
       </c>
       <c r="C116">
         <v>125</v>
@@ -11676,9 +11966,8 @@
       <c r="A117" t="s">
         <v>130</v>
       </c>
-      <c r="B117" t="str">
-        <f>CONCATENATE(LEFT(A117,5),"_",RIGHT(A117,2))</f>
-        <v>GRSPB_31</v>
+      <c r="B117" t="s">
+        <v>268</v>
       </c>
       <c r="C117">
         <v>125</v>
@@ -11769,9 +12058,8 @@
       <c r="A118" t="s">
         <v>131</v>
       </c>
-      <c r="B118" t="str">
-        <f t="shared" ref="B118:B127" si="2">CONCATENATE(LEFT(A118,5),"_",RIGHT(A118,2))</f>
-        <v>GRSPB_32</v>
+      <c r="B118" t="s">
+        <v>269</v>
       </c>
       <c r="C118">
         <v>123</v>
@@ -11862,9 +12150,8 @@
       <c r="A119" t="s">
         <v>132</v>
       </c>
-      <c r="B119" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_33</v>
+      <c r="B119" t="s">
+        <v>270</v>
       </c>
       <c r="C119">
         <v>123</v>
@@ -11955,9 +12242,8 @@
       <c r="A120" t="s">
         <v>133</v>
       </c>
-      <c r="B120" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_34</v>
+      <c r="B120" t="s">
+        <v>271</v>
       </c>
       <c r="C120">
         <v>123</v>
@@ -12048,9 +12334,8 @@
       <c r="A121" t="s">
         <v>134</v>
       </c>
-      <c r="B121" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_35</v>
+      <c r="B121" t="s">
+        <v>272</v>
       </c>
       <c r="C121">
         <v>123</v>
@@ -12141,9 +12426,8 @@
       <c r="A122" t="s">
         <v>135</v>
       </c>
-      <c r="B122" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_36</v>
+      <c r="B122" t="s">
+        <v>273</v>
       </c>
       <c r="C122">
         <v>125</v>
@@ -12234,9 +12518,8 @@
       <c r="A123" t="s">
         <v>136</v>
       </c>
-      <c r="B123" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_37</v>
+      <c r="B123" t="s">
+        <v>274</v>
       </c>
       <c r="C123">
         <v>125</v>
@@ -12327,9 +12610,8 @@
       <c r="A124" t="s">
         <v>137</v>
       </c>
-      <c r="B124" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_39</v>
+      <c r="B124" t="s">
+        <v>275</v>
       </c>
       <c r="C124">
         <v>129</v>
@@ -12420,9 +12702,8 @@
       <c r="A125" t="s">
         <v>138</v>
       </c>
-      <c r="B125" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_41</v>
+      <c r="B125" t="s">
+        <v>276</v>
       </c>
       <c r="C125">
         <v>123</v>
@@ -12513,9 +12794,8 @@
       <c r="A126" t="s">
         <v>139</v>
       </c>
-      <c r="B126" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_44</v>
+      <c r="B126" t="s">
+        <v>277</v>
       </c>
       <c r="C126">
         <v>123</v>
@@ -12606,9 +12886,8 @@
       <c r="A127" t="s">
         <v>140</v>
       </c>
-      <c r="B127" t="str">
-        <f t="shared" si="2"/>
-        <v>GRSPB_46</v>
+      <c r="B127" t="s">
+        <v>278</v>
       </c>
       <c r="C127">
         <v>123</v>
@@ -12699,9 +12978,8 @@
       <c r="A128" t="s">
         <v>141</v>
       </c>
-      <c r="B128" t="str">
-        <f>CONCATENATE(LEFT(A128,5),"_",RIGHT(A128,2))</f>
-        <v>GRSPB_49</v>
+      <c r="B128" t="s">
+        <v>279</v>
       </c>
       <c r="C128">
         <v>123</v>
@@ -12792,9 +13070,8 @@
       <c r="A129" t="s">
         <v>142</v>
       </c>
-      <c r="B129" t="str">
-        <f>CONCATENATE(LEFT(A129,4),"_",RIGHT(A129,2))</f>
-        <v>TBLR_01</v>
+      <c r="B129" t="s">
+        <v>280</v>
       </c>
       <c r="C129">
         <v>125</v>
@@ -12885,9 +13162,8 @@
       <c r="A130" t="s">
         <v>143</v>
       </c>
-      <c r="B130" t="str">
-        <f t="shared" ref="B130:B136" si="3">CONCATENATE(LEFT(A130,4),"_",RIGHT(A130,2))</f>
-        <v>TBLR_02</v>
+      <c r="B130" t="s">
+        <v>281</v>
       </c>
       <c r="C130">
         <v>123</v>
@@ -12978,9 +13254,8 @@
       <c r="A131" t="s">
         <v>144</v>
       </c>
-      <c r="B131" t="str">
-        <f t="shared" si="3"/>
-        <v>TBLR_03</v>
+      <c r="B131" t="s">
+        <v>282</v>
       </c>
       <c r="C131">
         <v>125</v>
@@ -13071,9 +13346,8 @@
       <c r="A132" t="s">
         <v>145</v>
       </c>
-      <c r="B132" t="str">
-        <f t="shared" si="3"/>
-        <v>TBLR_04</v>
+      <c r="B132" t="s">
+        <v>283</v>
       </c>
       <c r="C132">
         <v>125</v>
@@ -13164,9 +13438,8 @@
       <c r="A133" t="s">
         <v>146</v>
       </c>
-      <c r="B133" t="str">
-        <f t="shared" si="3"/>
-        <v>TBLR_05</v>
+      <c r="B133" t="s">
+        <v>284</v>
       </c>
       <c r="C133">
         <v>125</v>
@@ -13257,9 +13530,8 @@
       <c r="A134" t="s">
         <v>147</v>
       </c>
-      <c r="B134" t="str">
-        <f t="shared" si="3"/>
-        <v>TBLR_06</v>
+      <c r="B134" t="s">
+        <v>285</v>
       </c>
       <c r="C134">
         <v>125</v>
@@ -13350,9 +13622,8 @@
       <c r="A135" t="s">
         <v>148</v>
       </c>
-      <c r="B135" t="str">
-        <f t="shared" si="3"/>
-        <v>TBLR_07</v>
+      <c r="B135" t="s">
+        <v>286</v>
       </c>
       <c r="C135">
         <v>123</v>
@@ -13443,9 +13714,8 @@
       <c r="A136" t="s">
         <v>149</v>
       </c>
-      <c r="B136" t="str">
-        <f t="shared" si="3"/>
-        <v>TBLR_08</v>
+      <c r="B136" t="s">
+        <v>287</v>
       </c>
       <c r="C136">
         <v>123</v>

</xml_diff>

<commit_message>
analysis to impute total length alive of FER71, revisions
</commit_message>
<xml_diff>
--- a/raw_data/genotype_data.xlsx
+++ b/raw_data/genotype_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5FBC95-CCDF-9649-8C69-ACF955A9A7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557C2C77-BD21-6042-828B-8FBC206BB65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="13640" xr2:uid="{8655E8E0-4FE4-9C41-9F55-F43691CC9339}"/>
+    <workbookView xWindow="1040" yWindow="600" windowWidth="30060" windowHeight="13640" xr2:uid="{8655E8E0-4FE4-9C41-9F55-F43691CC9339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="290">
   <si>
     <t>sample_id</t>
   </si>
@@ -900,13 +900,19 @@
   </si>
   <si>
     <t>TBLR_08</t>
+  </si>
+  <si>
+    <t>FER71</t>
+  </si>
+  <si>
+    <t>FER_71</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -937,6 +943,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -958,13 +971,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BABEBB-635A-534D-90BA-1C6A4991D774}">
-  <dimension ref="A1:AD136"/>
+  <dimension ref="A1:AF137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11594,7 +11609,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -11686,7 +11701,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>127</v>
       </c>
@@ -11778,7 +11793,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>128</v>
       </c>
@@ -11870,7 +11885,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>129</v>
       </c>
@@ -11962,122 +11977,124 @@
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>288</v>
+      </c>
+      <c r="B117" t="s">
+        <v>289</v>
+      </c>
+      <c r="C117" s="6">
+        <v>123</v>
+      </c>
+      <c r="D117" s="6">
+        <v>123</v>
+      </c>
+      <c r="E117" s="6">
+        <v>196</v>
+      </c>
+      <c r="F117" s="6">
+        <v>200</v>
+      </c>
+      <c r="G117" s="6">
+        <v>167</v>
+      </c>
+      <c r="H117" s="6">
+        <v>167</v>
+      </c>
+      <c r="I117" s="6">
+        <v>102</v>
+      </c>
+      <c r="J117" s="6">
+        <v>108</v>
+      </c>
+      <c r="K117" s="6">
+        <v>146</v>
+      </c>
+      <c r="L117" s="6">
+        <v>148</v>
+      </c>
+      <c r="M117" s="6">
+        <v>105</v>
+      </c>
+      <c r="N117" s="6">
+        <v>117</v>
+      </c>
+      <c r="O117" s="6">
+        <v>198</v>
+      </c>
+      <c r="P117" s="6">
+        <v>198</v>
+      </c>
+      <c r="Q117" s="6">
+        <v>190</v>
+      </c>
+      <c r="R117" s="6">
+        <v>192</v>
+      </c>
+      <c r="S117" s="6">
+        <v>123</v>
+      </c>
+      <c r="T117" s="6">
+        <v>159</v>
+      </c>
+      <c r="U117" s="6">
+        <v>128</v>
+      </c>
+      <c r="V117" s="6">
+        <v>146</v>
+      </c>
+      <c r="W117" s="6">
+        <v>175</v>
+      </c>
+      <c r="X117" s="6">
+        <v>215</v>
+      </c>
+      <c r="Y117" s="6">
+        <v>104</v>
+      </c>
+      <c r="Z117" s="6">
+        <v>112</v>
+      </c>
+      <c r="AA117" s="6">
+        <v>158</v>
+      </c>
+      <c r="AB117" s="6">
+        <v>164</v>
+      </c>
+      <c r="AC117" s="6">
+        <v>124</v>
+      </c>
+      <c r="AD117" s="6">
+        <v>124</v>
+      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+    </row>
+    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>130</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" t="s">
         <v>268</v>
       </c>
-      <c r="C117">
+      <c r="C118">
         <v>125</v>
       </c>
-      <c r="D117">
+      <c r="D118">
         <v>129</v>
       </c>
-      <c r="E117">
-        <v>196</v>
-      </c>
-      <c r="F117">
+      <c r="E118">
+        <v>196</v>
+      </c>
+      <c r="F118">
         <v>200</v>
-      </c>
-      <c r="G117">
-        <v>163</v>
-      </c>
-      <c r="H117">
-        <v>163</v>
-      </c>
-      <c r="I117">
-        <v>102</v>
-      </c>
-      <c r="J117">
-        <v>102</v>
-      </c>
-      <c r="K117">
-        <v>148</v>
-      </c>
-      <c r="L117">
-        <v>148</v>
-      </c>
-      <c r="M117">
-        <v>117</v>
-      </c>
-      <c r="N117">
-        <v>119</v>
-      </c>
-      <c r="O117">
-        <v>184</v>
-      </c>
-      <c r="P117">
-        <v>184</v>
-      </c>
-      <c r="Q117">
-        <v>194</v>
-      </c>
-      <c r="R117">
-        <v>196</v>
-      </c>
-      <c r="S117">
-        <v>147</v>
-      </c>
-      <c r="T117">
-        <v>157</v>
-      </c>
-      <c r="U117">
-        <v>142</v>
-      </c>
-      <c r="V117">
-        <v>148</v>
-      </c>
-      <c r="W117">
-        <v>175</v>
-      </c>
-      <c r="X117">
-        <v>233</v>
-      </c>
-      <c r="Y117">
-        <v>110</v>
-      </c>
-      <c r="Z117">
-        <v>128</v>
-      </c>
-      <c r="AA117">
-        <v>158</v>
-      </c>
-      <c r="AB117">
-        <v>158</v>
-      </c>
-      <c r="AC117">
-        <v>110</v>
-      </c>
-      <c r="AD117">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>131</v>
-      </c>
-      <c r="B118" t="s">
-        <v>269</v>
-      </c>
-      <c r="C118">
-        <v>123</v>
-      </c>
-      <c r="D118">
-        <v>125</v>
-      </c>
-      <c r="E118">
-        <v>196</v>
-      </c>
-      <c r="F118">
-        <v>196</v>
       </c>
       <c r="G118">
         <v>163</v>
       </c>
       <c r="H118">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I118">
         <v>102</v>
@@ -12095,7 +12112,7 @@
         <v>117</v>
       </c>
       <c r="N118">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="O118">
         <v>184</v>
@@ -12104,72 +12121,72 @@
         <v>184</v>
       </c>
       <c r="Q118">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R118">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="S118">
+        <v>147</v>
+      </c>
+      <c r="T118">
+        <v>157</v>
+      </c>
+      <c r="U118">
+        <v>142</v>
+      </c>
+      <c r="V118">
+        <v>148</v>
+      </c>
+      <c r="W118">
         <v>175</v>
       </c>
-      <c r="T118">
-        <v>181</v>
-      </c>
-      <c r="U118">
-        <v>140</v>
-      </c>
-      <c r="V118">
-        <v>148</v>
-      </c>
-      <c r="W118">
-        <v>219</v>
-      </c>
       <c r="X118">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="Y118">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="Z118">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="AA118">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AB118">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="AC118">
         <v>110</v>
       </c>
       <c r="AD118">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B119" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C119">
         <v>123</v>
       </c>
       <c r="D119">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E119">
         <v>196</v>
       </c>
       <c r="F119">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G119">
         <v>163</v>
       </c>
       <c r="H119">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I119">
         <v>102</v>
@@ -12184,75 +12201,75 @@
         <v>148</v>
       </c>
       <c r="M119">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="N119">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="O119">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="P119">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="Q119">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="R119">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="S119">
         <v>175</v>
       </c>
       <c r="T119">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="U119">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V119">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="W119">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="X119">
-        <v>189</v>
+        <v>253</v>
       </c>
       <c r="Y119">
         <v>122</v>
       </c>
       <c r="Z119">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AA119">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="AB119">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="AC119">
         <v>110</v>
       </c>
       <c r="AD119">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B120" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C120">
         <v>123</v>
       </c>
       <c r="D120">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E120">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F120">
         <v>200</v>
@@ -12261,7 +12278,7 @@
         <v>163</v>
       </c>
       <c r="H120">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I120">
         <v>102</v>
@@ -12276,90 +12293,90 @@
         <v>148</v>
       </c>
       <c r="M120">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="N120">
         <v>117</v>
       </c>
       <c r="O120">
+        <v>198</v>
+      </c>
+      <c r="P120">
+        <v>198</v>
+      </c>
+      <c r="Q120">
         <v>194</v>
       </c>
-      <c r="P120">
-        <v>198</v>
-      </c>
-      <c r="Q120">
-        <v>190</v>
-      </c>
       <c r="R120">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="S120">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="T120">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="U120">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="V120">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="W120">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="X120">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="Y120">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="Z120">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="AA120">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AB120">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="AC120">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="AD120">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C121">
         <v>123</v>
       </c>
       <c r="D121">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E121">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F121">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G121">
         <v>163</v>
       </c>
       <c r="H121">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I121">
         <v>102</v>
       </c>
       <c r="J121">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K121">
         <v>148</v>
@@ -12371,72 +12388,72 @@
         <v>117</v>
       </c>
       <c r="N121">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O121">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="P121">
         <v>198</v>
       </c>
       <c r="Q121">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R121">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="S121">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="T121">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="U121">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="V121">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="W121">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="X121">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="Y121">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Z121">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AA121">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AB121">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AC121">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AD121">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B122" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C122">
+        <v>123</v>
+      </c>
+      <c r="D122">
         <v>125</v>
       </c>
-      <c r="D122">
-        <v>129</v>
-      </c>
       <c r="E122">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F122">
         <v>202</v>
@@ -12445,16 +12462,16 @@
         <v>163</v>
       </c>
       <c r="H122">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I122">
         <v>102</v>
       </c>
       <c r="J122">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="K122">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L122">
         <v>148</v>
@@ -12463,81 +12480,81 @@
         <v>117</v>
       </c>
       <c r="N122">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="O122">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="P122">
         <v>198</v>
       </c>
       <c r="Q122">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="R122">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="S122">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="T122">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="U122">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="V122">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="W122">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="X122">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="Y122">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Z122">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AA122">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="AB122">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="AC122">
+        <v>118</v>
+      </c>
+      <c r="AD122">
         <v>126</v>
       </c>
-      <c r="AD122">
-        <v>130</v>
-      </c>
     </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B123" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C123">
         <v>125</v>
       </c>
       <c r="D123">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E123">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F123">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G123">
         <v>163</v>
       </c>
       <c r="H123">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I123">
         <v>102</v>
@@ -12549,87 +12566,87 @@
         <v>146</v>
       </c>
       <c r="L123">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M123">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="N123">
         <v>117</v>
       </c>
       <c r="O123">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="P123">
         <v>198</v>
       </c>
       <c r="Q123">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="R123">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="S123">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="T123">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="U123">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="V123">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="W123">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="X123">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="Y123">
+        <v>114</v>
+      </c>
+      <c r="Z123">
         <v>120</v>
-      </c>
-      <c r="Z123">
-        <v>126</v>
       </c>
       <c r="AA123">
         <v>158</v>
       </c>
       <c r="AB123">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="AC123">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="AD123">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B124" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C124">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D124">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E124">
         <v>196</v>
       </c>
       <c r="F124">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G124">
         <v>163</v>
       </c>
       <c r="H124">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I124">
         <v>102</v>
@@ -12638,16 +12655,16 @@
         <v>102</v>
       </c>
       <c r="K124">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L124">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M124">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="N124">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O124">
         <v>194</v>
@@ -12659,54 +12676,54 @@
         <v>194</v>
       </c>
       <c r="R124">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="S124">
         <v>125</v>
       </c>
       <c r="T124">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="U124">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="V124">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="W124">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="X124">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="Y124">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="Z124">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="AA124">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="AB124">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="AC124">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AD124">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B125" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C125">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D125">
         <v>129</v>
@@ -12721,13 +12738,13 @@
         <v>163</v>
       </c>
       <c r="H125">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I125">
         <v>102</v>
       </c>
       <c r="J125">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K125">
         <v>148</v>
@@ -12739,63 +12756,63 @@
         <v>117</v>
       </c>
       <c r="N125">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="O125">
         <v>194</v>
       </c>
       <c r="P125">
+        <v>198</v>
+      </c>
+      <c r="Q125">
         <v>194</v>
       </c>
-      <c r="Q125">
-        <v>190</v>
-      </c>
       <c r="R125">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="S125">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="T125">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="U125">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="V125">
         <v>140</v>
       </c>
       <c r="W125">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="X125">
-        <v>241</v>
+        <v>205</v>
       </c>
       <c r="Y125">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="Z125">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="AA125">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AB125">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="AC125">
         <v>120</v>
       </c>
       <c r="AD125">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C126">
         <v>123</v>
@@ -12810,16 +12827,16 @@
         <v>196</v>
       </c>
       <c r="G126">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H126">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I126">
         <v>102</v>
       </c>
       <c r="J126">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K126">
         <v>148</v>
@@ -12828,10 +12845,10 @@
         <v>148</v>
       </c>
       <c r="M126">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="N126">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O126">
         <v>194</v>
@@ -12840,66 +12857,66 @@
         <v>194</v>
       </c>
       <c r="Q126">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="R126">
-        <v>196</v>
-      </c>
-      <c r="S126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="T126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="U126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="V126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="W126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="X126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="Y126" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z126" s="2" t="s">
-        <v>150</v>
+        <v>190</v>
+      </c>
+      <c r="S126">
+        <v>121</v>
+      </c>
+      <c r="T126">
+        <v>123</v>
+      </c>
+      <c r="U126">
+        <v>124</v>
+      </c>
+      <c r="V126">
+        <v>140</v>
+      </c>
+      <c r="W126">
+        <v>197</v>
+      </c>
+      <c r="X126">
+        <v>241</v>
+      </c>
+      <c r="Y126">
+        <v>104</v>
+      </c>
+      <c r="Z126">
+        <v>112</v>
       </c>
       <c r="AA126">
         <v>164</v>
       </c>
       <c r="AB126">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AC126">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AD126">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="127" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B127" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C127">
         <v>123</v>
       </c>
       <c r="D127">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E127">
         <v>196</v>
       </c>
       <c r="F127">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G127">
         <v>167</v>
@@ -12914,170 +12931,170 @@
         <v>102</v>
       </c>
       <c r="K127">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L127">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M127">
         <v>105</v>
       </c>
       <c r="N127">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O127">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="P127">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="Q127">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="R127">
         <v>196</v>
       </c>
-      <c r="S127">
-        <v>125</v>
-      </c>
-      <c r="T127">
-        <v>141</v>
-      </c>
-      <c r="U127">
-        <v>146</v>
-      </c>
-      <c r="V127">
+      <c r="S127" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="W127">
-        <v>197</v>
-      </c>
-      <c r="X127">
-        <v>225</v>
-      </c>
-      <c r="Y127">
-        <v>122</v>
-      </c>
-      <c r="Z127">
-        <v>126</v>
+      <c r="T127" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="U127" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="V127" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="W127" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="X127" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y127" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z127" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="AA127">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="AB127">
         <v>168</v>
       </c>
       <c r="AC127">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="AD127">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B128" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C128">
         <v>123</v>
       </c>
       <c r="D128">
+        <v>125</v>
+      </c>
+      <c r="E128">
+        <v>196</v>
+      </c>
+      <c r="F128">
+        <v>200</v>
+      </c>
+      <c r="G128">
+        <v>167</v>
+      </c>
+      <c r="H128">
+        <v>167</v>
+      </c>
+      <c r="I128">
+        <v>102</v>
+      </c>
+      <c r="J128">
+        <v>102</v>
+      </c>
+      <c r="K128">
+        <v>146</v>
+      </c>
+      <c r="L128">
+        <v>146</v>
+      </c>
+      <c r="M128">
+        <v>105</v>
+      </c>
+      <c r="N128">
         <v>129</v>
-      </c>
-      <c r="E128">
-        <v>196</v>
-      </c>
-      <c r="F128">
-        <v>196</v>
-      </c>
-      <c r="G128">
-        <v>163</v>
-      </c>
-      <c r="H128">
-        <v>163</v>
-      </c>
-      <c r="I128">
-        <v>102</v>
-      </c>
-      <c r="J128">
-        <v>106</v>
-      </c>
-      <c r="K128">
-        <v>148</v>
-      </c>
-      <c r="L128">
-        <v>148</v>
-      </c>
-      <c r="M128">
-        <v>117</v>
-      </c>
-      <c r="N128">
-        <v>117</v>
       </c>
       <c r="O128">
         <v>184</v>
       </c>
       <c r="P128">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="Q128">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="R128">
         <v>196</v>
       </c>
       <c r="S128">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="T128">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="U128">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="V128">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="W128">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="X128">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="Y128">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="Z128">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AA128">
         <v>158</v>
       </c>
       <c r="AB128">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="AC128">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="AD128">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B129" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C129">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D129">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E129">
         <v>196</v>
@@ -13086,10 +13103,10 @@
         <v>196</v>
       </c>
       <c r="G129">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H129">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I129">
         <v>102</v>
@@ -13098,10 +13115,10 @@
         <v>106</v>
       </c>
       <c r="K129">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L129">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M129">
         <v>117</v>
@@ -13119,54 +13136,54 @@
         <v>194</v>
       </c>
       <c r="R129">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="S129">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="T129">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="U129">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="V129">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W129">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="X129">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="Y129">
         <v>108</v>
       </c>
       <c r="Z129">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="AA129">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AB129">
         <v>164</v>
       </c>
       <c r="AC129">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="AD129">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B130" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C130">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D130">
         <v>125</v>
@@ -13175,19 +13192,19 @@
         <v>196</v>
       </c>
       <c r="F130">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G130">
         <v>167</v>
       </c>
       <c r="H130">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I130">
         <v>102</v>
       </c>
       <c r="J130">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K130">
         <v>146</v>
@@ -13196,43 +13213,43 @@
         <v>146</v>
       </c>
       <c r="M130">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="N130">
         <v>117</v>
       </c>
       <c r="O130">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="P130">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="Q130">
         <v>194</v>
       </c>
       <c r="R130">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="S130">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="T130">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="U130">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="V130">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="W130">
-        <v>235</v>
+        <v>175</v>
       </c>
       <c r="X130">
-        <v>265</v>
+        <v>189</v>
       </c>
       <c r="Y130">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="Z130">
         <v>120</v>
@@ -13241,24 +13258,24 @@
         <v>164</v>
       </c>
       <c r="AB130">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="AC130">
         <v>126</v>
       </c>
       <c r="AD130">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B131" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C131">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D131">
         <v>125</v>
@@ -13267,7 +13284,7 @@
         <v>196</v>
       </c>
       <c r="F131">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G131">
         <v>167</v>
@@ -13282,10 +13299,10 @@
         <v>102</v>
       </c>
       <c r="K131">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L131">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M131">
         <v>105</v>
@@ -13294,78 +13311,78 @@
         <v>117</v>
       </c>
       <c r="O131">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="P131">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="Q131">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="R131">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="S131">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="T131">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="U131">
+        <v>124</v>
+      </c>
+      <c r="V131">
         <v>126</v>
       </c>
-      <c r="V131">
-        <v>146</v>
-      </c>
       <c r="W131">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="X131">
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="Y131">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="Z131">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AA131">
         <v>164</v>
       </c>
       <c r="AB131">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AC131">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="AD131">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B132" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C132">
         <v>125</v>
       </c>
       <c r="D132">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E132">
         <v>196</v>
       </c>
       <c r="F132">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G132">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H132">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I132">
         <v>102</v>
@@ -13374,72 +13391,72 @@
         <v>102</v>
       </c>
       <c r="K132">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L132">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M132">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="N132">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O132">
         <v>184</v>
       </c>
       <c r="P132">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q132">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="R132">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="S132">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="T132">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="U132">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="V132">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W132">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="X132">
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="Y132">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="Z132">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="AA132">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="AB132">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AC132">
         <v>114</v>
       </c>
       <c r="AD132">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B133" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C133">
         <v>125</v>
@@ -13466,34 +13483,34 @@
         <v>102</v>
       </c>
       <c r="K133">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L133">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M133">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N133">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="O133">
         <v>184</v>
       </c>
       <c r="P133">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="Q133">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="R133">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="S133">
         <v>139</v>
       </c>
       <c r="T133">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="U133">
         <v>146</v>
@@ -13502,42 +13519,42 @@
         <v>148</v>
       </c>
       <c r="W133">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="X133">
-        <v>211</v>
+        <v>265</v>
       </c>
       <c r="Y133">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Z133">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AA133">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="AB133">
         <v>174</v>
       </c>
       <c r="AC133">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AD133">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B134" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C134">
         <v>125</v>
       </c>
       <c r="D134">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E134">
         <v>196</v>
@@ -13555,7 +13572,7 @@
         <v>102</v>
       </c>
       <c r="J134">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K134">
         <v>148</v>
@@ -13564,84 +13581,84 @@
         <v>148</v>
       </c>
       <c r="M134">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="N134">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O134">
         <v>184</v>
       </c>
       <c r="P134">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q134">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="R134">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="S134">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="T134">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="U134">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="V134">
         <v>148</v>
       </c>
       <c r="W134">
-        <v>215</v>
+        <v>189</v>
       </c>
       <c r="X134">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="Y134">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Z134">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AA134">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="AB134">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="AC134">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="AD134">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B135" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C135">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D135">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E135">
+        <v>196</v>
+      </c>
+      <c r="F135">
         <v>200</v>
-      </c>
-      <c r="F135">
-        <v>202</v>
       </c>
       <c r="G135">
         <v>163</v>
       </c>
       <c r="H135">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I135">
         <v>102</v>
@@ -13656,72 +13673,72 @@
         <v>148</v>
       </c>
       <c r="M135">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="N135">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="O135">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="P135">
         <v>198</v>
       </c>
       <c r="Q135">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="R135">
         <v>194</v>
       </c>
       <c r="S135">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="T135">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="U135">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="V135">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="W135">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="X135">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="Y135">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="Z135">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="AA135">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="AB135">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AC135">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AD135">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B136" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C136">
         <v>123</v>
       </c>
       <c r="D136">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E136">
         <v>200</v>
@@ -13733,43 +13750,43 @@
         <v>163</v>
       </c>
       <c r="H136">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I136">
         <v>102</v>
       </c>
       <c r="J136">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K136">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L136">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M136">
         <v>117</v>
       </c>
       <c r="N136">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O136">
+        <v>198</v>
+      </c>
+      <c r="P136">
+        <v>198</v>
+      </c>
+      <c r="Q136">
         <v>190</v>
       </c>
-      <c r="P136">
-        <v>198</v>
-      </c>
-      <c r="Q136">
-        <v>192</v>
-      </c>
       <c r="R136">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="S136">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="T136">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="U136">
         <v>146</v>
@@ -13778,13 +13795,13 @@
         <v>146</v>
       </c>
       <c r="W136">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="X136">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="Y136">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="Z136">
         <v>120</v>
@@ -13793,12 +13810,104 @@
         <v>164</v>
       </c>
       <c r="AB136">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="AC136">
         <v>120</v>
       </c>
       <c r="AD136">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>149</v>
+      </c>
+      <c r="B137" t="s">
+        <v>287</v>
+      </c>
+      <c r="C137">
+        <v>123</v>
+      </c>
+      <c r="D137">
+        <v>125</v>
+      </c>
+      <c r="E137">
+        <v>200</v>
+      </c>
+      <c r="F137">
+        <v>202</v>
+      </c>
+      <c r="G137">
+        <v>163</v>
+      </c>
+      <c r="H137">
+        <v>167</v>
+      </c>
+      <c r="I137">
+        <v>102</v>
+      </c>
+      <c r="J137">
+        <v>108</v>
+      </c>
+      <c r="K137">
+        <v>146</v>
+      </c>
+      <c r="L137">
+        <v>146</v>
+      </c>
+      <c r="M137">
+        <v>117</v>
+      </c>
+      <c r="N137">
+        <v>121</v>
+      </c>
+      <c r="O137">
+        <v>190</v>
+      </c>
+      <c r="P137">
+        <v>198</v>
+      </c>
+      <c r="Q137">
+        <v>192</v>
+      </c>
+      <c r="R137">
+        <v>196</v>
+      </c>
+      <c r="S137">
+        <v>143</v>
+      </c>
+      <c r="T137">
+        <v>165</v>
+      </c>
+      <c r="U137">
+        <v>146</v>
+      </c>
+      <c r="V137">
+        <v>146</v>
+      </c>
+      <c r="W137">
+        <v>189</v>
+      </c>
+      <c r="X137">
+        <v>189</v>
+      </c>
+      <c r="Y137">
+        <v>102</v>
+      </c>
+      <c r="Z137">
+        <v>120</v>
+      </c>
+      <c r="AA137">
+        <v>164</v>
+      </c>
+      <c r="AB137">
+        <v>174</v>
+      </c>
+      <c r="AC137">
+        <v>120</v>
+      </c>
+      <c r="AD137">
         <v>124</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edited structure numbers for genepop/structure files
</commit_message>
<xml_diff>
--- a/raw_data/genotype_data.xlsx
+++ b/raw_data/genotype_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557C2C77-BD21-6042-828B-8FBC206BB65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01CD9D4-1C93-0443-BB04-60DCB0905381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="600" windowWidth="30060" windowHeight="13640" xr2:uid="{8655E8E0-4FE4-9C41-9F55-F43691CC9339}"/>
+    <workbookView xWindow="5120" yWindow="500" windowWidth="28800" windowHeight="13640" xr2:uid="{8655E8E0-4FE4-9C41-9F55-F43691CC9339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -842,77 +842,77 @@
     <t>FER_70</t>
   </si>
   <si>
-    <t>GRSPB_31</t>
-  </si>
-  <si>
-    <t>GRSPB_32</t>
-  </si>
-  <si>
-    <t>GRSPB_33</t>
-  </si>
-  <si>
-    <t>GRSPB_34</t>
-  </si>
-  <si>
-    <t>GRSPB_35</t>
-  </si>
-  <si>
-    <t>GRSPB_36</t>
-  </si>
-  <si>
-    <t>GRSPB_37</t>
-  </si>
-  <si>
-    <t>GRSPB_39</t>
-  </si>
-  <si>
-    <t>GRSPB_41</t>
-  </si>
-  <si>
-    <t>GRSPB_44</t>
-  </si>
-  <si>
-    <t>GRSPB_46</t>
-  </si>
-  <si>
-    <t>GRSPB_49</t>
-  </si>
-  <si>
-    <t>TBLR_01</t>
-  </si>
-  <si>
-    <t>TBLR_02</t>
-  </si>
-  <si>
-    <t>TBLR_03</t>
-  </si>
-  <si>
-    <t>TBLR_04</t>
-  </si>
-  <si>
-    <t>TBLR_05</t>
-  </si>
-  <si>
-    <t>TBLR_06</t>
-  </si>
-  <si>
-    <t>TBLR_07</t>
-  </si>
-  <si>
-    <t>TBLR_08</t>
-  </si>
-  <si>
     <t>FER71</t>
   </si>
   <si>
     <t>FER_71</t>
+  </si>
+  <si>
+    <t>REF_01</t>
+  </si>
+  <si>
+    <t>REF_02</t>
+  </si>
+  <si>
+    <t>REF_03</t>
+  </si>
+  <si>
+    <t>REF_04</t>
+  </si>
+  <si>
+    <t>REF_05</t>
+  </si>
+  <si>
+    <t>REF_06</t>
+  </si>
+  <si>
+    <t>REF_07</t>
+  </si>
+  <si>
+    <t>REF_08</t>
+  </si>
+  <si>
+    <t>REF_09</t>
+  </si>
+  <si>
+    <t>REF_10</t>
+  </si>
+  <si>
+    <t>REF_11</t>
+  </si>
+  <si>
+    <t>REF_12</t>
+  </si>
+  <si>
+    <t>REF_13</t>
+  </si>
+  <si>
+    <t>REF_14</t>
+  </si>
+  <si>
+    <t>REF_15</t>
+  </si>
+  <si>
+    <t>REF_16</t>
+  </si>
+  <si>
+    <t>REF_17</t>
+  </si>
+  <si>
+    <t>REF_18</t>
+  </si>
+  <si>
+    <t>REF_19</t>
+  </si>
+  <si>
+    <t>REF_20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -950,6 +950,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -971,15 +977,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BABEBB-635A-534D-90BA-1C6A4991D774}">
-  <dimension ref="A1:AF137"/>
+  <dimension ref="A1:AD137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118:B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11609,7 +11614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -11701,7 +11706,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>127</v>
       </c>
@@ -11793,7 +11798,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>128</v>
       </c>
@@ -11885,7 +11890,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>129</v>
       </c>
@@ -11977,12 +11982,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="B117" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C117" s="6">
         <v>123</v>
@@ -12068,15 +12073,13 @@
       <c r="AD117" s="6">
         <v>124</v>
       </c>
-      <c r="AE117" s="7"/>
-      <c r="AF117" s="7"/>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>130</v>
       </c>
       <c r="B118" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C118">
         <v>125</v>
@@ -12163,12 +12166,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>131</v>
       </c>
       <c r="B119" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C119">
         <v>123</v>
@@ -12255,12 +12258,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>132</v>
       </c>
       <c r="B120" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C120">
         <v>123</v>
@@ -12347,12 +12350,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C121">
         <v>123</v>
@@ -12439,12 +12442,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>134</v>
       </c>
       <c r="B122" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C122">
         <v>123</v>
@@ -12531,12 +12534,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>135</v>
       </c>
       <c r="B123" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C123">
         <v>125</v>
@@ -12623,12 +12626,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>136</v>
       </c>
       <c r="B124" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C124">
         <v>125</v>
@@ -12715,12 +12718,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>137</v>
       </c>
       <c r="B125" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C125">
         <v>129</v>
@@ -12807,12 +12810,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C126">
         <v>123</v>
@@ -12899,12 +12902,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>139</v>
       </c>
       <c r="B127" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C127">
         <v>123</v>
@@ -12991,12 +12994,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>140</v>
       </c>
       <c r="B128" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C128">
         <v>123</v>
@@ -13088,7 +13091,7 @@
         <v>141</v>
       </c>
       <c r="B129" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C129">
         <v>123</v>
@@ -13180,7 +13183,7 @@
         <v>142</v>
       </c>
       <c r="B130" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C130">
         <v>125</v>
@@ -13272,7 +13275,7 @@
         <v>143</v>
       </c>
       <c r="B131" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C131">
         <v>123</v>
@@ -13364,7 +13367,7 @@
         <v>144</v>
       </c>
       <c r="B132" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C132">
         <v>125</v>
@@ -13456,7 +13459,7 @@
         <v>145</v>
       </c>
       <c r="B133" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C133">
         <v>125</v>
@@ -13548,7 +13551,7 @@
         <v>146</v>
       </c>
       <c r="B134" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C134">
         <v>125</v>
@@ -13640,7 +13643,7 @@
         <v>147</v>
       </c>
       <c r="B135" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C135">
         <v>125</v>
@@ -13732,7 +13735,7 @@
         <v>148</v>
       </c>
       <c r="B136" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C136">
         <v>123</v>
@@ -13824,7 +13827,7 @@
         <v>149</v>
       </c>
       <c r="B137" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C137">
         <v>123</v>
@@ -13912,6 +13915,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>